<commit_message>
Finished exceptions for sets and cards
</commit_message>
<xml_diff>
--- a/card_exceptions.xlsx
+++ b/card_exceptions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629E1717-2073-4766-87E9-5E616A7EA1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B327EB-F711-48D8-B527-1E2873944553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="157">
   <si>
     <t>Old Set</t>
   </si>
@@ -73,21 +73,12 @@
     <t>From the Vault: Lore</t>
   </si>
   <si>
-    <t>162</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Lord of Shatterskull Pass</t>
   </si>
   <si>
     <t>Release Event Promos</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>Rise of the Eldrazi Promos</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>Dictate of the Twin Gods</t>
   </si>
   <si>
-    <t>41</t>
-  </si>
-  <si>
     <t>Journey into Nyx Promos</t>
   </si>
   <si>
@@ -112,81 +100,39 @@
     <t>Buy-a-Box Promos</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
     <t>Magic Origins Promos</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>Endbringer</t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
     <t>Oath of the Gatewatch Promos</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Necropolis Fiend</t>
   </si>
   <si>
     <t>Clash Pack Promos</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>Fate Reforged Clash Pack</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Hero's Downfall</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Sultai Ascendancy</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>Reaper of the Wilds</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Whip of Erebos</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Courser of Kruphix</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Sultai Charm</t>
   </si>
   <si>
@@ -196,48 +142,24 @@
     <t>Khans of Tarkir Promos</t>
   </si>
   <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
     <t>Archfiend of Ifnir</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>Amonkhet Promos</t>
   </si>
   <si>
-    <t>78</t>
-  </si>
-  <si>
     <t>Rienne, Angel of Rebirth</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
     <t>Core Set 2020</t>
   </si>
   <si>
-    <t>281</t>
-  </si>
-  <si>
     <t>Gilded Lotus</t>
   </si>
   <si>
     <t>Promo Pack: Core Set 2020</t>
   </si>
   <si>
-    <t>118</t>
-  </si>
-  <si>
     <t>Dominaria Promos</t>
   </si>
   <si>
@@ -253,15 +175,9 @@
     <t>Throne of Eldraine</t>
   </si>
   <si>
-    <t>396</t>
-  </si>
-  <si>
     <t>Wishclaw Talisman</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
     <t>Throne of Eldraine Promos</t>
   </si>
   <si>
@@ -271,33 +187,21 @@
     <t>Emry, Lurker of the Loch</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>43p</t>
   </si>
   <si>
     <t>Athreos, Shroud-Veiled</t>
   </si>
   <si>
-    <t>54</t>
-  </si>
-  <si>
     <t>Theros Beyond Death</t>
   </si>
   <si>
-    <t>269</t>
-  </si>
-  <si>
     <t>Atris, Oracle of Half-Truths</t>
   </si>
   <si>
     <t>Prerelease Cards</t>
   </si>
   <si>
-    <t>1473</t>
-  </si>
-  <si>
     <t>Theros Beyond Death Promos</t>
   </si>
   <si>
@@ -310,9 +214,6 @@
     <t>Promo Pack: Theros Beyond Death</t>
   </si>
   <si>
-    <t>354</t>
-  </si>
-  <si>
     <t>Underworld Breach</t>
   </si>
   <si>
@@ -322,9 +223,6 @@
     <t>Emergent Ultimatum</t>
   </si>
   <si>
-    <t>1531</t>
-  </si>
-  <si>
     <t>Ikoria: Lair of Behemoths Promos</t>
   </si>
   <si>
@@ -337,33 +235,21 @@
     <t>Promo Pack: Ikoria</t>
   </si>
   <si>
-    <t>56</t>
-  </si>
-  <si>
     <t>221p</t>
   </si>
   <si>
     <t>Keruga, the Macrosage</t>
   </si>
   <si>
-    <t>59</t>
-  </si>
-  <si>
     <t>225p</t>
   </si>
   <si>
     <t>Chord of Calling</t>
   </si>
   <si>
-    <t>1644</t>
-  </si>
-  <si>
     <t>Double Masters</t>
   </si>
   <si>
-    <t>384</t>
-  </si>
-  <si>
     <t>Thieving Skydiver</t>
   </si>
   <si>
@@ -379,33 +265,21 @@
     <t>Skyclave Relic</t>
   </si>
   <si>
-    <t>71</t>
-  </si>
-  <si>
     <t>252p</t>
   </si>
   <si>
     <t>Sengir, the Dark Baron</t>
   </si>
   <si>
-    <t>1729</t>
-  </si>
-  <si>
     <t>Commander Legends</t>
   </si>
   <si>
-    <t>722</t>
-  </si>
-  <si>
     <t>Realmwalker</t>
   </si>
   <si>
     <t>Kaldheim</t>
   </si>
   <si>
-    <t>399</t>
-  </si>
-  <si>
     <t>Kenrith, the Returned King (Non-Foil)</t>
   </si>
   <si>
@@ -415,18 +289,12 @@
     <t>Kenrith, the Returned King</t>
   </si>
   <si>
-    <t>303</t>
-  </si>
-  <si>
     <t>Culling Ritual</t>
   </si>
   <si>
     <t>Promo Pack: Strixhaven</t>
   </si>
   <si>
-    <t>62</t>
-  </si>
-  <si>
     <t>Strixhaven: School of Mages Promos</t>
   </si>
   <si>
@@ -442,84 +310,21 @@
     <t>Modern Horizons 2</t>
   </si>
   <si>
-    <t>492</t>
-  </si>
-  <si>
     <t>Plains</t>
   </si>
   <si>
-    <t>594</t>
-  </si>
-  <si>
-    <t>481</t>
-  </si>
-  <si>
-    <t>595</t>
-  </si>
-  <si>
-    <t>482</t>
-  </si>
-  <si>
     <t>Island</t>
   </si>
   <si>
-    <t>596</t>
-  </si>
-  <si>
-    <t>483</t>
-  </si>
-  <si>
-    <t>597</t>
-  </si>
-  <si>
-    <t>484</t>
-  </si>
-  <si>
     <t>Swamp</t>
   </si>
   <si>
-    <t>598</t>
-  </si>
-  <si>
-    <t>485</t>
-  </si>
-  <si>
-    <t>599</t>
-  </si>
-  <si>
-    <t>486</t>
-  </si>
-  <si>
     <t>Mountain</t>
   </si>
   <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>487</t>
-  </si>
-  <si>
-    <t>601</t>
-  </si>
-  <si>
-    <t>488</t>
-  </si>
-  <si>
     <t>Forest</t>
   </si>
   <si>
-    <t>602</t>
-  </si>
-  <si>
-    <t>489</t>
-  </si>
-  <si>
-    <t>603</t>
-  </si>
-  <si>
-    <t>490</t>
-  </si>
-  <si>
     <t>Prosperous Innkeeper</t>
   </si>
   <si>
@@ -529,9 +334,6 @@
     <t>Adventures in the Forgotten Realms</t>
   </si>
   <si>
-    <t>402</t>
-  </si>
-  <si>
     <t>Dig Through Time</t>
   </si>
   <si>
@@ -565,9 +367,6 @@
     <t>Promo Pack: Innistrad Midnight Hunt</t>
   </si>
   <si>
-    <t>63</t>
-  </si>
-  <si>
     <t>Innistrad: Midnight Hunt Promos</t>
   </si>
   <si>
@@ -577,21 +376,12 @@
     <t>Voldaren Estate</t>
   </si>
   <si>
-    <t>66</t>
-  </si>
-  <si>
     <t>Innistrad: Crimson Vow</t>
   </si>
   <si>
-    <t>403</t>
-  </si>
-  <si>
     <t>Tatsunari, Toad Rider</t>
   </si>
   <si>
-    <t>2284</t>
-  </si>
-  <si>
     <t>Kamigawa: Neon Dynasty Promos</t>
   </si>
   <si>
@@ -601,9 +391,6 @@
     <t>Satoru Umezawa</t>
   </si>
   <si>
-    <t>2317</t>
-  </si>
-  <si>
     <t>234s</t>
   </si>
   <si>
@@ -613,30 +400,18 @@
     <t>Promo Pack: Kamigawa</t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
     <t>153s</t>
   </si>
   <si>
     <t>Jaxis, the Troublemaker</t>
   </si>
   <si>
-    <t>68</t>
-  </si>
-  <si>
     <t>Streets of New Capenna</t>
   </si>
   <si>
-    <t>461</t>
-  </si>
-  <si>
     <t>Astarion, the Decadent</t>
   </si>
   <si>
-    <t>2474</t>
-  </si>
-  <si>
     <t>Battle for Baldur's Gate Promos</t>
   </si>
   <si>
@@ -646,21 +421,12 @@
     <t>Herd Migration</t>
   </si>
   <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>Dominaria United</t>
   </si>
   <si>
-    <t>429</t>
-  </si>
-  <si>
     <t>Blackcleave Cliffs</t>
   </si>
   <si>
-    <t>2750</t>
-  </si>
-  <si>
     <t>Phyrexia: All Will Be One Promos</t>
   </si>
   <si>
@@ -670,15 +436,9 @@
     <t>Ghalta and Mavren</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>March of the Machine</t>
   </si>
   <si>
-    <t>386</t>
-  </si>
-  <si>
     <t>Inga and Esika</t>
   </si>
   <si>
@@ -704,6 +464,33 @@
   </si>
   <si>
     <t>The Brothers' War</t>
+  </si>
+  <si>
+    <t>The Brothers' War Promos</t>
+  </si>
+  <si>
+    <t>Deathbloom Ritualist</t>
+  </si>
+  <si>
+    <t>208p</t>
+  </si>
+  <si>
+    <t>Fabricate</t>
+  </si>
+  <si>
+    <t>Warhammer 40,000 Commander</t>
+  </si>
+  <si>
+    <t>Maestros Diabolist</t>
+  </si>
+  <si>
+    <t>Promo Pack: Streets of New Capenna</t>
+  </si>
+  <si>
+    <t>200p</t>
+  </si>
+  <si>
+    <t>Streets of New Capenna Promos</t>
   </si>
 </sst>
 </file>
@@ -780,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -788,6 +575,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,18 +867,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1092,7 +888,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1101,7 +897,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -1115,14 +911,14 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>61</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>79</v>
       </c>
       <c r="G2" s="1"/>
@@ -1134,14 +930,14 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>162</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>11</v>
       </c>
       <c r="G3" s="1"/>
@@ -1153,12 +949,12 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>82</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
@@ -1170,12 +966,12 @@
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5">
         <v>16</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="1" t="b">
         <v>1</v>
       </c>
@@ -1187,224 +983,224 @@
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
+      <c r="C6" s="5">
+        <v>162</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
+      <c r="F6" s="5">
+        <v>11</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="5">
+        <v>24</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="5">
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="5">
+        <v>25</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="F9" s="5">
+        <v>29</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="5">
+        <v>49</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="C11" s="5">
+        <v>7</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="C12" s="5">
+        <v>8</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="5">
+        <v>9</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="F13" s="5">
+        <v>3</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="C14" s="5">
+        <v>10</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
+      </c>
+      <c r="F14" s="5">
+        <v>4</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="C15" s="5">
+        <v>11</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
+      </c>
+      <c r="F15" s="5">
+        <v>5</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
+      </c>
+      <c r="C16" s="5">
+        <v>12</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
+      </c>
+      <c r="F16" s="5">
+        <v>6</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
+      </c>
+      <c r="F17" s="5">
+        <v>204</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -1415,1526 +1211,1556 @@
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>59</v>
+      <c r="C18" s="5">
+        <v>61</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>60</v>
+      <c r="F18" s="5">
+        <v>79</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
+      </c>
+      <c r="C19" s="5">
+        <v>32</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
+      </c>
+      <c r="F19" s="5">
+        <v>78</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="C20" s="5">
+        <v>52</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
+      </c>
+      <c r="F20" s="5">
+        <v>281</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>45</v>
+      </c>
+      <c r="C21" s="5">
+        <v>118</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>73</v>
+        <v>46</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
+      </c>
+      <c r="F22" s="5">
+        <v>396</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>79</v>
+        <v>49</v>
+      </c>
+      <c r="C23" s="5">
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>81</v>
+        <v>52</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>49</v>
+      </c>
+      <c r="C24" s="5">
+        <v>17</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>84</v>
+        <v>52</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>25</v>
+      </c>
+      <c r="C25" s="5">
+        <v>54</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>88</v>
+        <v>57</v>
+      </c>
+      <c r="F25" s="5">
+        <v>269</v>
       </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>59</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1473</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>93</v>
+        <v>60</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>96</v>
+        <v>57</v>
+      </c>
+      <c r="F27" s="5">
+        <v>354</v>
       </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>63</v>
+      </c>
+      <c r="C28" s="5">
+        <v>41</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>98</v>
+        <v>60</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>100</v>
+        <v>59</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1531</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>102</v>
+        <v>67</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>105</v>
+        <v>70</v>
+      </c>
+      <c r="C30" s="5">
+        <v>56</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>106</v>
+        <v>67</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>108</v>
+        <v>70</v>
+      </c>
+      <c r="C31" s="5">
+        <v>59</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>109</v>
+        <v>67</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>111</v>
+        <v>59</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1644</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>113</v>
+        <v>75</v>
+      </c>
+      <c r="F32" s="5">
+        <v>384</v>
       </c>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
+      </c>
+      <c r="C33" s="5">
+        <v>25</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>117</v>
+        <v>78</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>119</v>
+        <v>77</v>
+      </c>
+      <c r="C34" s="5">
+        <v>71</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>120</v>
+        <v>78</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>122</v>
+        <v>59</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1729</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>124</v>
+        <v>83</v>
+      </c>
+      <c r="F35" s="5">
+        <v>722</v>
       </c>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>25</v>
+      </c>
+      <c r="C36" s="5">
+        <v>59</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>127</v>
+        <v>85</v>
+      </c>
+      <c r="F36" s="5">
+        <v>399</v>
       </c>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>25</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>131</v>
+        <v>50</v>
+      </c>
+      <c r="F37" s="5">
+        <v>303</v>
       </c>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>134</v>
+        <v>90</v>
+      </c>
+      <c r="C38" s="5">
+        <v>62</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>136</v>
+        <v>91</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>94</v>
+      </c>
+      <c r="C39" s="5">
+        <v>9</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>140</v>
+        <v>95</v>
+      </c>
+      <c r="F39" s="5">
+        <v>492</v>
       </c>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>142</v>
+        <v>95</v>
+      </c>
+      <c r="C40" s="5">
+        <v>594</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1" t="s">
-        <v>143</v>
+      <c r="F40" s="5">
+        <v>481</v>
       </c>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>144</v>
+        <v>95</v>
+      </c>
+      <c r="C41" s="5">
+        <v>595</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="1" t="s">
-        <v>145</v>
+      <c r="F41" s="5">
+        <v>482</v>
       </c>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>147</v>
+        <v>95</v>
+      </c>
+      <c r="C42" s="5">
+        <v>596</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="1" t="s">
-        <v>148</v>
+      <c r="F42" s="5">
+        <v>483</v>
       </c>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>149</v>
+        <v>95</v>
+      </c>
+      <c r="C43" s="5">
+        <v>597</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1" t="s">
-        <v>150</v>
+      <c r="F43" s="5">
+        <v>484</v>
       </c>
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>152</v>
+        <v>95</v>
+      </c>
+      <c r="C44" s="5">
+        <v>598</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1" t="s">
-        <v>153</v>
+      <c r="F44" s="5">
+        <v>485</v>
       </c>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>154</v>
+        <v>95</v>
+      </c>
+      <c r="C45" s="5">
+        <v>599</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1" t="s">
-        <v>155</v>
+      <c r="F45" s="5">
+        <v>486</v>
       </c>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>157</v>
+        <v>95</v>
+      </c>
+      <c r="C46" s="5">
+        <v>600</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1" t="s">
-        <v>158</v>
+      <c r="F46" s="5">
+        <v>487</v>
       </c>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>159</v>
+        <v>95</v>
+      </c>
+      <c r="C47" s="5">
+        <v>601</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1" t="s">
-        <v>160</v>
+      <c r="F47" s="5">
+        <v>488</v>
       </c>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>162</v>
+        <v>95</v>
+      </c>
+      <c r="C48" s="5">
+        <v>602</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1" t="s">
-        <v>163</v>
+      <c r="F48" s="5">
+        <v>489</v>
       </c>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>164</v>
+        <v>95</v>
+      </c>
+      <c r="C49" s="5">
+        <v>603</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="1" t="s">
-        <v>165</v>
+      <c r="F49" s="5">
+        <v>490</v>
       </c>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>51</v>
+        <v>102</v>
+      </c>
+      <c r="C50" s="5">
+        <v>5</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>169</v>
+        <v>103</v>
+      </c>
+      <c r="F50" s="5">
+        <v>402</v>
       </c>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>49</v>
+        <v>105</v>
+      </c>
+      <c r="C51" s="5">
+        <v>4</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>44</v>
+        <v>106</v>
+      </c>
+      <c r="F51" s="5">
+        <v>2</v>
       </c>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>51</v>
+        <v>105</v>
+      </c>
+      <c r="C52" s="5">
+        <v>5</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>36</v>
+        <v>106</v>
+      </c>
+      <c r="F52" s="5">
+        <v>3</v>
       </c>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>54</v>
+        <v>109</v>
+      </c>
+      <c r="C53" s="5">
+        <v>6</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>41</v>
+        <v>110</v>
+      </c>
+      <c r="F53" s="5">
+        <v>1</v>
       </c>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>51</v>
+        <v>110</v>
+      </c>
+      <c r="F54" s="5">
+        <v>5</v>
       </c>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>181</v>
+        <v>114</v>
+      </c>
+      <c r="C55" s="5">
+        <v>63</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>183</v>
+        <v>115</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>184</v>
+        <v>117</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>185</v>
+        <v>25</v>
+      </c>
+      <c r="C56" s="5">
+        <v>66</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>187</v>
+        <v>118</v>
+      </c>
+      <c r="F56" s="5">
+        <v>403</v>
       </c>
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>189</v>
+        <v>59</v>
+      </c>
+      <c r="C57" s="5">
+        <v>2284</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>191</v>
+        <v>120</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>193</v>
+        <v>59</v>
+      </c>
+      <c r="C58" s="5">
+        <v>2317</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>194</v>
+        <v>120</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>197</v>
+        <v>125</v>
+      </c>
+      <c r="C59" s="5">
+        <v>39</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>198</v>
+        <v>120</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>199</v>
+        <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>200</v>
+        <v>25</v>
+      </c>
+      <c r="C60" s="5">
+        <v>68</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>202</v>
+        <v>128</v>
+      </c>
+      <c r="F60" s="5">
+        <v>461</v>
       </c>
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>203</v>
+        <v>129</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>204</v>
+        <v>59</v>
+      </c>
+      <c r="C61" s="5">
+        <v>2474</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>206</v>
+        <v>130</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>207</v>
+        <v>132</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>208</v>
+        <v>94</v>
+      </c>
+      <c r="C62" s="5">
+        <v>70</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>210</v>
+        <v>133</v>
+      </c>
+      <c r="F62" s="5">
+        <v>429</v>
       </c>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>212</v>
+        <v>59</v>
+      </c>
+      <c r="C63" s="5">
+        <v>2750</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>214</v>
+        <v>135</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>215</v>
+        <v>137</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>216</v>
+        <v>94</v>
+      </c>
+      <c r="C64" s="5">
+        <v>23</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>218</v>
+        <v>138</v>
+      </c>
+      <c r="F64" s="5">
+        <v>386</v>
       </c>
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>219</v>
+        <v>139</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>221</v>
+        <v>140</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="F65" s="5"/>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" s="1">
+        <v>18</v>
+      </c>
+      <c r="C66" s="5">
         <v>24</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C67" s="1">
+        <v>105</v>
+      </c>
+      <c r="C67" s="5">
         <v>4</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F67" s="1">
+        <v>106</v>
+      </c>
+      <c r="F67" s="5">
         <v>2</v>
       </c>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C68" s="1">
+        <v>105</v>
+      </c>
+      <c r="C68" s="5">
         <v>5</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F68" s="1">
+        <v>106</v>
+      </c>
+      <c r="F68" s="5">
         <v>3</v>
       </c>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>223</v>
+        <v>143</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C69" s="1">
+        <v>105</v>
+      </c>
+      <c r="C69" s="5">
         <v>1</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F69" s="1">
-        <v>1</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="F69" s="5"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>225</v>
+        <v>145</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C70" s="1">
+        <v>146</v>
+      </c>
+      <c r="C70" s="5">
         <v>381</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F70" s="1">
-        <v>381</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="F70" s="5"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+      <c r="E71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F71" s="5"/>
       <c r="G71" s="1"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="5">
+        <v>41</v>
+      </c>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="5">
+        <v>181</v>
+      </c>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="E73" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F73" s="5"/>
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="E74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F74" s="5"/>
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="C75" s="5"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+      <c r="F75" s="5"/>
       <c r="G75" s="1"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="C76" s="5"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="F76" s="5"/>
       <c r="G76" s="1"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="C77" s="5"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="5"/>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="C78" s="5"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="F78" s="5"/>
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="C79" s="5"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="F79" s="5"/>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="C80" s="5"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
+      <c r="F80" s="5"/>
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="C81" s="5"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
+      <c r="F81" s="5"/>
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
+      <c r="C82" s="5"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
+      <c r="F82" s="5"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="C83" s="5"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
+      <c r="F83" s="5"/>
       <c r="G83" s="1"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
+      <c r="C84" s="5"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="F84" s="5"/>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
+      <c r="C85" s="5"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+      <c r="F85" s="5"/>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
+      <c r="C86" s="5"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+      <c r="F86" s="5"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
+      <c r="C87" s="5"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
+      <c r="F87" s="5"/>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
+      <c r="C88" s="5"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
+      <c r="F88" s="5"/>
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
+      <c r="C89" s="5"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
+      <c r="F89" s="5"/>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
+      <c r="C90" s="5"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
+      <c r="F90" s="5"/>
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="C91" s="5"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
+      <c r="F91" s="5"/>
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
+      <c r="C92" s="5"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
+      <c r="F92" s="5"/>
       <c r="G92" s="1"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
+      <c r="C93" s="5"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
+      <c r="F93" s="5"/>
       <c r="G93" s="1"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="C94" s="5"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
+      <c r="F94" s="5"/>
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
+      <c r="C95" s="5"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
+      <c r="F95" s="5"/>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="C96" s="5"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
+      <c r="F96" s="5"/>
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
+      <c r="C97" s="5"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
+      <c r="F97" s="5"/>
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="C98" s="5"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
+      <c r="F98" s="5"/>
       <c r="G98" s="1"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="C99" s="5"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
+      <c r="F99" s="5"/>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="C100" s="5"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
+      <c r="F100" s="5"/>
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="C101" s="5"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
+      <c r="F101" s="5"/>
       <c r="G101" s="1"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
+      <c r="C102" s="5"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
+      <c r="F102" s="5"/>
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
+      <c r="C103" s="5"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
+      <c r="F103" s="5"/>
       <c r="G103" s="1"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
+      <c r="C104" s="5"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
+      <c r="F104" s="5"/>
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
+      <c r="C105" s="5"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
+      <c r="F105" s="5"/>
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
+      <c r="C106" s="5"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
+      <c r="F106" s="5"/>
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
+      <c r="C107" s="5"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
+      <c r="F107" s="5"/>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
+      <c r="C108" s="5"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
+      <c r="F108" s="5"/>
       <c r="G108" s="1"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
+      <c r="C109" s="5"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
+      <c r="F109" s="5"/>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
+      <c r="C110" s="5"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
+      <c r="F110" s="5"/>
       <c r="G110" s="1"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
+      <c r="C111" s="5"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
+      <c r="F111" s="5"/>
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
+      <c r="C112" s="5"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
+      <c r="F112" s="5"/>
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
+      <c r="C113" s="5"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
+      <c r="F113" s="5"/>
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
+      <c r="C114" s="5"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
+      <c r="F114" s="5"/>
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
+      <c r="C115" s="5"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
+      <c r="F115" s="5"/>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
+      <c r="C116" s="5"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
+      <c r="F116" s="5"/>
       <c r="G116" s="1"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
+      <c r="C117" s="5"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
+      <c r="F117" s="5"/>
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
+      <c r="C118" s="5"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
+      <c r="F118" s="5"/>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
+      <c r="C119" s="5"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
+      <c r="F119" s="5"/>
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
+      <c r="C120" s="5"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
+      <c r="F120" s="5"/>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
+      <c r="C121" s="5"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
+      <c r="F121" s="5"/>
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
+      <c r="C122" s="5"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
+      <c r="F122" s="5"/>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
+      <c r="C123" s="5"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
+      <c r="F123" s="5"/>
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
+      <c r="C124" s="5"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
+      <c r="F124" s="5"/>
       <c r="G124" s="1"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
+      <c r="C125" s="5"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
+      <c r="F125" s="5"/>
       <c r="G125" s="1"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
+      <c r="C126" s="5"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
+      <c r="F126" s="5"/>
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
+      <c r="C127" s="5"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="1"/>
+      <c r="F127" s="5"/>
       <c r="G127" s="1"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
+      <c r="C128" s="5"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="1"/>
+      <c r="F128" s="5"/>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
+      <c r="C129" s="5"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
+      <c r="F129" s="5"/>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
+      <c r="C130" s="5"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
-      <c r="F130" s="1"/>
+      <c r="F130" s="5"/>
       <c r="G130" s="1"/>
     </row>
   </sheetData>

</xml_diff>